<commit_message>
Mouse click to jump. Before enabling web build
</commit_message>
<xml_diff>
--- a/Business/FinancialPlan.xlsx
+++ b/Business/FinancialPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Documents\Apps\Phoenix\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C07E29A-F172-4146-9DDB-DC8EAE763C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28035A9-6875-4B7F-B382-B2C822C47D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{990BFE11-CA5B-4A46-A56F-9B3285507C10}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>Project Virgo Financial Plan</t>
   </si>
@@ -247,6 +247,27 @@
   </si>
   <si>
     <t>Percent Competion</t>
+  </si>
+  <si>
+    <t>Target Dates</t>
+  </si>
+  <si>
+    <t>Need funding by</t>
+  </si>
+  <si>
+    <t>Game shippable by</t>
+  </si>
+  <si>
+    <t>Game playable by</t>
+  </si>
+  <si>
+    <t>Game released by</t>
+  </si>
+  <si>
+    <t>Trying to get something playable in half time time I have to get funding.</t>
+  </si>
+  <si>
+    <t>Fully 1.5 year estimated timeline</t>
   </si>
 </sst>
 </file>
@@ -422,7 +443,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -465,6 +486,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -781,15 +803,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E837B8-03A2-4787-92C0-8A69DADFB706}">
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" customWidth="1"/>
@@ -2725,13 +2747,14 @@
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="26">
         <f t="shared" si="11"/>
-        <v>0.44748858447488582</v>
+        <v>0.44871794871795079</v>
       </c>
       <c r="B95" t="s">
         <v>58</v>
       </c>
       <c r="C95" s="5">
-        <v>44746</v>
+        <f>D4</f>
+        <v>44746.673076923078</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2787,6 +2810,66 @@
       </c>
       <c r="C104" s="2">
         <v>45049</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B107" s="27"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>18</v>
+      </c>
+      <c r="B108" s="2">
+        <f>A4</f>
+        <v>44501</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>72</v>
+      </c>
+      <c r="B109" s="2">
+        <f>D4</f>
+        <v>44746.673076923078</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>75</v>
+      </c>
+      <c r="B111" s="2">
+        <f>C103</f>
+        <v>45048.5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="2"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>73</v>
+      </c>
+      <c r="B113" s="2">
+        <f>B109</f>
+        <v>44746.673076923078</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>74</v>
+      </c>
+      <c r="B114" s="2">
+        <f>B108+(B109-B108)*0.5</f>
+        <v>44623.836538461539</v>
+      </c>
+      <c r="C114" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fly shadow in water. Terrain gen
</commit_message>
<xml_diff>
--- a/Business/FinancialPlan.xlsx
+++ b/Business/FinancialPlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Documents\Apps\Phoenix\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28035A9-6875-4B7F-B382-B2C822C47D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28431F29-33A0-4473-928F-B3910ED32285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{990BFE11-CA5B-4A46-A56F-9B3285507C10}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="83">
   <si>
     <t>Project Virgo Financial Plan</t>
   </si>
@@ -255,19 +255,34 @@
     <t>Need funding by</t>
   </si>
   <si>
-    <t>Game shippable by</t>
-  </si>
-  <si>
-    <t>Game playable by</t>
-  </si>
-  <si>
     <t>Game released by</t>
   </si>
   <si>
-    <t>Trying to get something playable in half time time I have to get funding.</t>
-  </si>
-  <si>
     <t>Fully 1.5 year estimated timeline</t>
+  </si>
+  <si>
+    <t>Community demo build</t>
+  </si>
+  <si>
+    <t>Get people in the game!</t>
+  </si>
+  <si>
+    <t>Demo Playable by</t>
+  </si>
+  <si>
+    <t>Game MVP</t>
+  </si>
+  <si>
+    <t>Enough to make another game</t>
+  </si>
+  <si>
+    <t>Enough to make another game and take a nice vacation</t>
+  </si>
+  <si>
+    <t>Anything past this goes to wildlife / environmental charity</t>
+  </si>
+  <si>
+    <t>This might be more than I know what to do with</t>
   </si>
 </sst>
 </file>
@@ -803,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E837B8-03A2-4787-92C0-8A69DADFB706}">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,17 +1697,21 @@
         <v>57.00748847926269</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="3">
+        <f>SUM(G13:G16)</f>
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>22</v>
       </c>
@@ -1710,7 +1729,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>9.99</v>
       </c>
@@ -1729,12 +1748,12 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
         <v>26</v>
       </c>
@@ -1759,7 +1778,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>1000</v>
       </c>
@@ -1789,7 +1808,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>2000</v>
       </c>
@@ -1819,7 +1838,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>3000</v>
       </c>
@@ -1849,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>4000</v>
       </c>
@@ -1879,7 +1898,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>5000</v>
       </c>
@@ -1909,7 +1928,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>6000</v>
       </c>
@@ -1939,7 +1958,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>7000</v>
       </c>
@@ -1969,7 +1988,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>8000</v>
       </c>
@@ -1999,7 +2018,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>9000</v>
       </c>
@@ -2029,7 +2048,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>10000</v>
       </c>
@@ -2058,7 +2077,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>15000</v>
       </c>
@@ -2087,7 +2106,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
         <v>20000</v>
       </c>
@@ -2117,8 +2136,11 @@
         <v>400</v>
       </c>
       <c r="I51" s="20"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>25000</v>
       </c>
@@ -2147,7 +2169,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
         <v>30000</v>
       </c>
@@ -2177,8 +2199,11 @@
         <v>600</v>
       </c>
       <c r="I53" s="24"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>35000</v>
       </c>
@@ -2207,7 +2232,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>40000</v>
       </c>
@@ -2236,7 +2261,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>45000</v>
       </c>
@@ -2265,36 +2290,41 @@
         <v>900</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="22">
         <v>50000</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="23">
         <f t="shared" si="4"/>
         <v>499500</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="23">
         <f t="shared" si="5"/>
         <v>349650</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="23">
         <f t="shared" si="6"/>
         <v>244754.99999999997</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E57" s="23">
         <f t="shared" si="3"/>
         <v>34399.999999999869</v>
       </c>
-      <c r="F57" s="3">
+      <c r="F57" s="23">
         <f t="shared" si="7"/>
         <v>210355.00000000012</v>
       </c>
-      <c r="H57" s="16">
+      <c r="G57" s="24"/>
+      <c r="H57" s="25">
         <f t="shared" si="8"/>
         <v>1000</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="24"/>
+      <c r="J57" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>60000</v>
       </c>
@@ -2323,36 +2353,41 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="13">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="18">
         <v>70000</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="19">
         <f t="shared" si="4"/>
         <v>699300</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="19">
         <f t="shared" si="5"/>
         <v>489509.99999999994</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="19">
         <f t="shared" si="6"/>
         <v>342656.99999999994</v>
       </c>
-      <c r="E59" s="3">
+      <c r="E59" s="19">
         <f t="shared" si="3"/>
         <v>34399.999999999869</v>
       </c>
-      <c r="F59" s="3">
+      <c r="F59" s="19">
         <f t="shared" si="7"/>
         <v>308257.00000000006</v>
       </c>
-      <c r="H59" s="16">
+      <c r="G59" s="20"/>
+      <c r="H59" s="21">
         <f t="shared" si="8"/>
         <v>1400</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="20"/>
+      <c r="J59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>80000</v>
       </c>
@@ -2381,7 +2416,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>90000</v>
       </c>
@@ -2410,7 +2445,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>100000</v>
       </c>
@@ -2439,7 +2474,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>200000</v>
       </c>
@@ -2468,7 +2503,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>300000</v>
       </c>
@@ -2697,9 +2732,20 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
-      <c r="B87" s="7"/>
-      <c r="C87" s="15"/>
+      <c r="A87" s="26">
+        <f t="shared" si="11"/>
+        <v>0.22435897435897539</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87" s="15">
+        <f>B109</f>
+        <v>44623.836538461539</v>
+      </c>
+      <c r="D87" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="26"/>
@@ -2758,7 +2804,17 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="26"/>
+      <c r="A96" s="26">
+        <f t="shared" si="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>78</v>
+      </c>
+      <c r="C96" s="2">
+        <f>B111</f>
+        <v>44774.75</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="26"/>
@@ -2829,47 +2885,44 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>77</v>
+      </c>
+      <c r="B109" s="2">
+        <f>B108+(B110-B108)*0.5</f>
+        <v>44623.836538461539</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>72</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B110" s="2">
         <f>D4</f>
         <v>44746.673076923078</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B111" s="2">
+        <f>B108+(B115-B108)*0.5</f>
+        <v>44774.75</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="2"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>73</v>
+      </c>
+      <c r="B115" s="2">
         <f>C103</f>
         <v>45048.5</v>
       </c>
-      <c r="C111" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>73</v>
-      </c>
-      <c r="B113" s="2">
-        <f>B109</f>
-        <v>44746.673076923078</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="C115" t="s">
         <v>74</v>
-      </c>
-      <c r="B114" s="2">
-        <f>B108+(B109-B108)*0.5</f>
-        <v>44623.836538461539</v>
-      </c>
-      <c r="C114" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
About to change from circuitry puzzle to flight puzzle primarily
</commit_message>
<xml_diff>
--- a/Business/FinancialPlan.xlsx
+++ b/Business/FinancialPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael\Documents\Apps\Phoenix\Business\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89C8855-5373-4F56-BA16-8696CB0086E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF27C65-36FC-4DD1-99FC-71BE90527F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{990BFE11-CA5B-4A46-A56F-9B3285507C10}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Project Virgo Financial Plan</t>
   </si>
@@ -292,6 +292,12 @@
   </si>
   <si>
     <t>Charity goal</t>
+  </si>
+  <si>
+    <t>Went out in public for first time and got public to play test</t>
+  </si>
+  <si>
+    <t>Public testing Demo v0.3</t>
   </si>
 </sst>
 </file>
@@ -857,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E837B8-03A2-4787-92C0-8A69DADFB706}">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2893,7 +2899,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="26">
         <f t="shared" si="13"/>
         <v>4.3835616438356165E-2</v>
@@ -2908,7 +2914,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="26">
         <f t="shared" si="13"/>
         <v>4.3835616438356165E-2</v>
@@ -2923,7 +2929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="26">
         <f t="shared" si="13"/>
         <v>7.6712328767123292E-2</v>
@@ -2938,7 +2944,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="26">
         <f t="shared" si="13"/>
         <v>8.9497716894977167E-2</v>
@@ -2953,7 +2959,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="26">
         <f t="shared" si="13"/>
         <v>9.8630136986301367E-2</v>
@@ -2968,7 +2974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="26">
         <f t="shared" si="13"/>
         <v>0.12237442922374429</v>
@@ -2983,7 +2989,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="26">
         <f t="shared" si="13"/>
         <v>0.22435897435897539</v>
@@ -2999,37 +3005,54 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="15"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="26">
+        <f t="shared" si="13"/>
+        <v>0.26484018264840181</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C88" s="15">
+        <v>44646</v>
+      </c>
+      <c r="D88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="26"/>
       <c r="B89" s="7"/>
       <c r="C89" s="15"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G89" s="3">
+        <v>5487.1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="26"/>
       <c r="B90" s="7"/>
       <c r="C90" s="15"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="26"/>
       <c r="B91" s="7"/>
       <c r="C91" s="15"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="26"/>
       <c r="B92" s="7"/>
       <c r="C92" s="15"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="26"/>
       <c r="B93" s="7"/>
       <c r="C93" s="15"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G93" s="3">
+        <f>G89-G105</f>
+        <v>3622.1000000000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="26">
         <f t="shared" si="13"/>
         <v>0.33333333333333331</v>
@@ -3041,8 +3064,11 @@
         <f>C79+6*B32</f>
         <v>44683.5</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G94" s="3">
+        <v>1733.33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="26">
         <f t="shared" si="13"/>
         <v>0.44871794871795079</v>
@@ -3054,8 +3080,16 @@
         <f>D4</f>
         <v>44746.673076923078</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <f>G93/G94</f>
+        <v>2.0896770955328763</v>
+      </c>
+      <c r="H95">
+        <f>G95*B32</f>
+        <v>63.561011655791653</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="26">
         <f t="shared" si="13"/>
         <v>0.5</v>
@@ -3067,35 +3101,39 @@
         <f>B111</f>
         <v>44774.75</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="H96" s="2">
+        <f ca="1">TODAY()+H95</f>
+        <v>44710.561011655795</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="26"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="26"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="26"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="26"/>
       <c r="B100" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="26"/>
       <c r="B101" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="26"/>
       <c r="B102" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="26">
         <f t="shared" si="13"/>
         <v>1</v>
@@ -3107,8 +3145,11 @@
         <f>C94+12*B32</f>
         <v>45048.5</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="26">
         <f t="shared" si="13"/>
         <v>1.0009132420091325</v>
@@ -3119,14 +3160,23 @@
       <c r="C104" s="2">
         <v>45049</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G105" s="3">
+        <f>G104+G103</f>
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="40" t="s">
         <v>69</v>
       </c>
       <c r="B107" s="27"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>18</v>
       </c>
@@ -3135,7 +3185,7 @@
         <v>44501</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>75</v>
       </c>
@@ -3144,7 +3194,7 @@
         <v>44623.836538461539</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>70</v>
       </c>
@@ -3153,7 +3203,7 @@
         <v>44746.673076923078</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>76</v>
       </c>
@@ -3162,7 +3212,7 @@
         <v>44774.75</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B112" s="2"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>